<commit_message>
Update latest data and find k's correlation. To-do: find case number's linkage
</commit_message>
<xml_diff>
--- a/doc/excels/correlation.xlsx
+++ b/doc/excels/correlation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="179">
   <si>
     <t>Population that can work from home</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>pp45</t>
+  </si>
+  <si>
+    <t>B_old</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2133,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3100,7 +3103,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5054,7 +5057,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6024,7 +6027,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6994,7 +6997,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7964,7 +7967,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12814,7 +12817,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13798,7 +13801,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14782,7 +14785,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15752,7 +15755,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>B_old</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -25562,16 +25565,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1390650</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26306,10 +26309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN114"/>
+  <dimension ref="A1:BO114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="BL7" sqref="BL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26318,9 +26321,10 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="39" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -26508,16 +26512,19 @@
         <v>167</v>
       </c>
       <c r="BL1" t="s">
+        <v>178</v>
+      </c>
+      <c r="BM1" t="s">
         <v>5</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>147</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -26729,14 +26736,17 @@
         <v>-0.83017995200000005</v>
       </c>
       <c r="BM2">
+        <v>-0.85555897949401305</v>
+      </c>
+      <c r="BN2">
         <f>-BL2</f>
         <v>0.83017995200000005</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <v>0.59318082599999999</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -26948,14 +26958,17 @@
         <v>-0.66275320500000001</v>
       </c>
       <c r="BM3">
-        <f t="shared" ref="BM3:BM66" si="12">-BL3</f>
+        <v>-0.755555951443313</v>
+      </c>
+      <c r="BN3">
+        <f t="shared" ref="BN3:BN66" si="12">-BL3</f>
         <v>0.66275320500000001</v>
       </c>
-      <c r="BN3">
+      <c r="BO3">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -27167,14 +27180,17 @@
         <v>-0.76478399600000002</v>
       </c>
       <c r="BM4">
+        <v>-0.79001646316755303</v>
+      </c>
+      <c r="BN4">
         <f t="shared" si="12"/>
         <v>0.76478399600000002</v>
       </c>
-      <c r="BN4">
+      <c r="BO4">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -27386,14 +27402,17 @@
         <v>-0.64159151199999997</v>
       </c>
       <c r="BM5">
+        <v>-0.68437366198278504</v>
+      </c>
+      <c r="BN5">
         <f t="shared" si="12"/>
         <v>0.64159151199999997</v>
       </c>
-      <c r="BN5">
+      <c r="BO5">
         <v>0.57657443600000002</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -27605,14 +27624,17 @@
         <v>-0.77641131900000004</v>
       </c>
       <c r="BM6">
+        <v>-0.79287304415406301</v>
+      </c>
+      <c r="BN6">
         <f t="shared" si="12"/>
         <v>0.77641131900000004</v>
       </c>
-      <c r="BN6">
+      <c r="BO6">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -27824,14 +27846,17 @@
         <v>-0.75167671700000005</v>
       </c>
       <c r="BM7">
+        <v>-0.82092831945325595</v>
+      </c>
+      <c r="BN7">
         <f t="shared" si="12"/>
         <v>0.75167671700000005</v>
       </c>
-      <c r="BN7">
+      <c r="BO7">
         <v>0.57521145299999998</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -28043,14 +28068,17 @@
         <v>-0.51119024899999999</v>
       </c>
       <c r="BM8">
+        <v>-0.57502094535020398</v>
+      </c>
+      <c r="BN8">
         <f t="shared" si="12"/>
         <v>0.51119024899999999</v>
       </c>
-      <c r="BN8">
+      <c r="BO8">
         <v>0.451402953</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -28262,14 +28290,17 @@
         <v>-0.717160346</v>
       </c>
       <c r="BM9">
+        <v>-0.76271528961788004</v>
+      </c>
+      <c r="BN9">
         <f t="shared" si="12"/>
         <v>0.717160346</v>
       </c>
-      <c r="BN9">
+      <c r="BO9">
         <v>0.44627200900000003</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -28481,14 +28512,17 @@
         <v>-0.80420622500000005</v>
       </c>
       <c r="BM10">
+        <v>-0.89658307870570997</v>
+      </c>
+      <c r="BN10">
         <f t="shared" si="12"/>
         <v>0.80420622500000005</v>
       </c>
-      <c r="BN10">
+      <c r="BO10">
         <v>0.51945645799999995</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -28700,14 +28734,17 @@
         <v>-0.63883321800000004</v>
       </c>
       <c r="BM11">
+        <v>-0.72305067638007203</v>
+      </c>
+      <c r="BN11">
         <f t="shared" si="12"/>
         <v>0.63883321800000004</v>
       </c>
-      <c r="BN11">
+      <c r="BO11">
         <v>0.52249942500000002</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -28919,14 +28956,17 @@
         <v>-0.79725182299999997</v>
       </c>
       <c r="BM12">
+        <v>-0.82739191107451104</v>
+      </c>
+      <c r="BN12">
         <f t="shared" si="12"/>
         <v>0.79725182299999997</v>
       </c>
-      <c r="BN12">
+      <c r="BO12">
         <v>0.59365532399999998</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -29138,14 +29178,17 @@
         <v>-0.86258183099999997</v>
       </c>
       <c r="BM13">
+        <v>-0.873917622295596</v>
+      </c>
+      <c r="BN13">
         <f t="shared" si="12"/>
         <v>0.86258183099999997</v>
       </c>
-      <c r="BN13">
+      <c r="BO13">
         <v>0.61497841200000003</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -29357,14 +29400,17 @@
         <v>-0.84766470199999999</v>
       </c>
       <c r="BM14">
+        <v>-0.87948653323542703</v>
+      </c>
+      <c r="BN14">
         <f t="shared" si="12"/>
         <v>0.84766470199999999</v>
       </c>
-      <c r="BN14">
+      <c r="BO14">
         <v>0.61497841200000003</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -29576,14 +29622,17 @@
         <v>-0.59570078999999998</v>
       </c>
       <c r="BM15">
+        <v>-0.61305106881724403</v>
+      </c>
+      <c r="BN15">
         <f t="shared" si="12"/>
         <v>0.59570078999999998</v>
       </c>
-      <c r="BN15">
+      <c r="BO15">
         <v>0.55997530900000003</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -29795,14 +29844,17 @@
         <v>-0.76965242899999997</v>
       </c>
       <c r="BM16">
+        <v>-0.750471802998393</v>
+      </c>
+      <c r="BN16">
         <f t="shared" si="12"/>
         <v>0.76965242899999997</v>
       </c>
-      <c r="BN16">
+      <c r="BO16">
         <v>0.54885689100000001</v>
       </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -30014,14 +30066,17 @@
         <v>-0.79136457900000001</v>
       </c>
       <c r="BM17">
+        <v>-0.79053712445317503</v>
+      </c>
+      <c r="BN17">
         <f t="shared" si="12"/>
         <v>0.79136457900000001</v>
       </c>
-      <c r="BN17">
+      <c r="BO17">
         <v>0.51736134499999997</v>
       </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -30233,14 +30288,17 @@
         <v>-0.72871449099999996</v>
       </c>
       <c r="BM18">
+        <v>-0.73903819220837697</v>
+      </c>
+      <c r="BN18">
         <f t="shared" si="12"/>
         <v>0.72871449099999996</v>
       </c>
-      <c r="BN18">
+      <c r="BO18">
         <v>0.48878642</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -30452,14 +30510,17 @@
         <v>-0.61134467100000001</v>
       </c>
       <c r="BM19">
+        <v>-0.64214359281525002</v>
+      </c>
+      <c r="BN19">
         <f t="shared" si="12"/>
         <v>0.61134467100000001</v>
       </c>
-      <c r="BN19">
+      <c r="BO19">
         <v>0.55598323699999996</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -30671,14 +30732,17 @@
         <v>-0.69339437599999998</v>
       </c>
       <c r="BM20">
+        <v>-0.72031929821428398</v>
+      </c>
+      <c r="BN20">
         <f t="shared" si="12"/>
         <v>0.69339437599999998</v>
       </c>
-      <c r="BN20">
+      <c r="BO20">
         <v>0.55598323699999996</v>
       </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -30890,14 +30954,17 @@
         <v>-0.63284876700000003</v>
       </c>
       <c r="BM21">
+        <v>-0.64137704401058104</v>
+      </c>
+      <c r="BN21">
         <f t="shared" si="12"/>
         <v>0.63284876700000003</v>
       </c>
-      <c r="BN21">
+      <c r="BO21">
         <v>0.53949475300000005</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -31109,14 +31176,17 @@
         <v>-0.659771828</v>
       </c>
       <c r="BM22">
+        <v>-0.718262058192355</v>
+      </c>
+      <c r="BN22">
         <f t="shared" si="12"/>
         <v>0.659771828</v>
       </c>
-      <c r="BN22">
+      <c r="BO22">
         <v>0.55459261900000001</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -31328,14 +31398,17 @@
         <v>-0.79277684100000001</v>
       </c>
       <c r="BM23">
+        <v>-0.81520404546804104</v>
+      </c>
+      <c r="BN23">
         <f t="shared" si="12"/>
         <v>0.79277684100000001</v>
       </c>
-      <c r="BN23">
+      <c r="BO23">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -31547,14 +31620,17 @@
         <v>-0.59346206700000004</v>
       </c>
       <c r="BM24">
+        <v>-0.56224213555044</v>
+      </c>
+      <c r="BN24">
         <f t="shared" si="12"/>
         <v>0.59346206700000004</v>
       </c>
-      <c r="BN24">
+      <c r="BO24">
         <v>0.46419387000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -31766,14 +31842,17 @@
         <v>-0.75776273800000005</v>
       </c>
       <c r="BM25">
+        <v>-0.79258348063423301</v>
+      </c>
+      <c r="BN25">
         <f t="shared" si="12"/>
         <v>0.75776273800000005</v>
       </c>
-      <c r="BN25">
+      <c r="BO25">
         <v>0.71935892800000001</v>
       </c>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -31985,14 +32064,17 @@
         <v>-0.55986519599999995</v>
       </c>
       <c r="BM26">
+        <v>-0.68787104676152799</v>
+      </c>
+      <c r="BN26">
         <f t="shared" si="12"/>
         <v>0.55986519599999995</v>
       </c>
-      <c r="BN26">
+      <c r="BO26">
         <v>0.44607749699999999</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -32204,14 +32286,17 @@
         <v>-0.597569197</v>
       </c>
       <c r="BM27">
+        <v>-0.67284304310798304</v>
+      </c>
+      <c r="BN27">
         <f t="shared" si="12"/>
         <v>0.597569197</v>
       </c>
-      <c r="BN27">
+      <c r="BO27">
         <v>0.71935892800000001</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -32423,14 +32508,17 @@
         <v>-0.73336292999999997</v>
       </c>
       <c r="BM28">
+        <v>-0.74429707716551796</v>
+      </c>
+      <c r="BN28">
         <f t="shared" si="12"/>
         <v>0.73336292999999997</v>
       </c>
-      <c r="BN28">
+      <c r="BO28">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -32642,14 +32730,17 @@
         <v>-0.62501819199999997</v>
       </c>
       <c r="BM29">
+        <v>-0.65121029265478603</v>
+      </c>
+      <c r="BN29">
         <f t="shared" si="12"/>
         <v>0.62501819199999997</v>
       </c>
-      <c r="BN29">
+      <c r="BO29">
         <v>0.52578006700000002</v>
       </c>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -32861,14 +32952,17 @@
         <v>-0.76991579700000001</v>
       </c>
       <c r="BM30">
+        <v>-0.77514603496173795</v>
+      </c>
+      <c r="BN30">
         <f t="shared" si="12"/>
         <v>0.76991579700000001</v>
       </c>
-      <c r="BN30">
+      <c r="BO30">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -33080,14 +33174,17 @@
         <v>-0.55500611899999996</v>
       </c>
       <c r="BM31">
+        <v>-0.57744717151053704</v>
+      </c>
+      <c r="BN31">
         <f t="shared" si="12"/>
         <v>0.55500611899999996</v>
       </c>
-      <c r="BN31">
+      <c r="BO31">
         <v>0.49033346500000002</v>
       </c>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -33299,14 +33396,17 @@
         <v>-0.76250190600000001</v>
       </c>
       <c r="BM32">
+        <v>-0.82498281181225597</v>
+      </c>
+      <c r="BN32">
         <f t="shared" si="12"/>
         <v>0.76250190600000001</v>
       </c>
-      <c r="BN32">
+      <c r="BO32">
         <v>0.56623688500000002</v>
       </c>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -33518,14 +33618,17 @@
         <v>-0.64324003600000002</v>
       </c>
       <c r="BM33">
+        <v>-0.64990443845139401</v>
+      </c>
+      <c r="BN33">
         <f t="shared" si="12"/>
         <v>0.64324003600000002</v>
       </c>
-      <c r="BN33">
+      <c r="BO33">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -33737,14 +33840,17 @@
         <v>-0.64571333200000003</v>
       </c>
       <c r="BM34">
+        <v>-0.68704591281090299</v>
+      </c>
+      <c r="BN34">
         <f t="shared" si="12"/>
         <v>0.64571333200000003</v>
       </c>
-      <c r="BN34">
+      <c r="BO34">
         <v>0.55598323699999996</v>
       </c>
     </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -33956,14 +34062,17 @@
         <v>-0.40958599699999998</v>
       </c>
       <c r="BM35">
+        <v>-0.66438185918417303</v>
+      </c>
+      <c r="BN35">
         <f t="shared" si="12"/>
         <v>0.40958599699999998</v>
       </c>
-      <c r="BN35">
+      <c r="BO35">
         <v>0.47984638699999999</v>
       </c>
     </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -34175,14 +34284,17 @@
         <v>-0.43374253000000002</v>
       </c>
       <c r="BM36">
+        <v>-0.37747763160236902</v>
+      </c>
+      <c r="BN36">
         <f t="shared" si="12"/>
         <v>0.43374253000000002</v>
       </c>
-      <c r="BN36">
+      <c r="BO36">
         <v>0.50351302399999998</v>
       </c>
     </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -34394,14 +34506,17 @@
         <v>-0.81961854199999995</v>
       </c>
       <c r="BM37">
+        <v>-0.82540644943096197</v>
+      </c>
+      <c r="BN37">
         <f t="shared" si="12"/>
         <v>0.81961854199999995</v>
       </c>
-      <c r="BN37">
+      <c r="BO37">
         <v>0.61497841200000003</v>
       </c>
     </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -34613,14 +34728,17 @@
         <v>-0.72288010300000005</v>
       </c>
       <c r="BM38">
+        <v>-0.74790088866902305</v>
+      </c>
+      <c r="BN38">
         <f t="shared" si="12"/>
         <v>0.72288010300000005</v>
       </c>
-      <c r="BN38">
+      <c r="BO38">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -34832,14 +34950,17 @@
         <v>-0.710802041</v>
       </c>
       <c r="BM39">
+        <v>-0.72600943267345797</v>
+      </c>
+      <c r="BN39">
         <f t="shared" si="12"/>
         <v>0.710802041</v>
       </c>
-      <c r="BN39">
+      <c r="BO39">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -35051,14 +35172,17 @@
         <v>-0.74388424200000003</v>
       </c>
       <c r="BM40">
+        <v>-0.75290772834275999</v>
+      </c>
+      <c r="BN40">
         <f t="shared" si="12"/>
         <v>0.74388424200000003</v>
       </c>
-      <c r="BN40">
+      <c r="BO40">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -35270,14 +35394,17 @@
         <v>-0.68039265400000004</v>
       </c>
       <c r="BM41">
+        <v>-0.72481047821373501</v>
+      </c>
+      <c r="BN41">
         <f t="shared" si="12"/>
         <v>0.68039265400000004</v>
       </c>
-      <c r="BN41">
+      <c r="BO41">
         <v>0.40215384900000001</v>
       </c>
     </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -35489,14 +35616,17 @@
         <v>-0.71164587800000001</v>
       </c>
       <c r="BM42">
+        <v>-0.74459434307942496</v>
+      </c>
+      <c r="BN42">
         <f t="shared" si="12"/>
         <v>0.71164587800000001</v>
       </c>
-      <c r="BN42">
+      <c r="BO42">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -35708,14 +35838,17 @@
         <v>-0.67624318100000003</v>
       </c>
       <c r="BM43">
+        <v>-0.70805263736329804</v>
+      </c>
+      <c r="BN43">
         <f t="shared" si="12"/>
         <v>0.67624318100000003</v>
       </c>
-      <c r="BN43">
+      <c r="BO43">
         <v>0.52022376999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -35927,14 +36060,17 @@
         <v>-0.58098067799999997</v>
       </c>
       <c r="BM44">
+        <v>-0.60911758706276697</v>
+      </c>
+      <c r="BN44">
         <f t="shared" si="12"/>
         <v>0.58098067799999997</v>
       </c>
-      <c r="BN44">
+      <c r="BO44">
         <v>0.495052347</v>
       </c>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -36146,14 +36282,17 @@
         <v>-0.89265086500000002</v>
       </c>
       <c r="BM45">
+        <v>-0.90332316756216802</v>
+      </c>
+      <c r="BN45">
         <f t="shared" si="12"/>
         <v>0.89265086500000002</v>
       </c>
-      <c r="BN45">
+      <c r="BO45">
         <v>0.617147997</v>
       </c>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -36365,14 +36504,17 @@
         <v>-0.48420986900000001</v>
       </c>
       <c r="BM46">
+        <v>-0.523029563975828</v>
+      </c>
+      <c r="BN46">
         <f t="shared" si="12"/>
         <v>0.48420986900000001</v>
       </c>
-      <c r="BN46">
+      <c r="BO46">
         <v>0.60592918600000001</v>
       </c>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -36584,14 +36726,17 @@
         <v>-0.78763895299999998</v>
       </c>
       <c r="BM47">
+        <v>-0.80677753553216602</v>
+      </c>
+      <c r="BN47">
         <f t="shared" si="12"/>
         <v>0.78763895299999998</v>
       </c>
-      <c r="BN47">
+      <c r="BO47">
         <v>0.57521145299999998</v>
       </c>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -36803,14 +36948,17 @@
         <v>-0.59668546499999997</v>
       </c>
       <c r="BM48">
+        <v>-0.57292808504246895</v>
+      </c>
+      <c r="BN48">
         <f t="shared" si="12"/>
         <v>0.59668546499999997</v>
       </c>
-      <c r="BN48">
+      <c r="BO48">
         <v>0.48780200699999998</v>
       </c>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -37022,14 +37170,17 @@
         <v>-0.56259338999999997</v>
       </c>
       <c r="BM49">
+        <v>-0.56667090594284797</v>
+      </c>
+      <c r="BN49">
         <f t="shared" si="12"/>
         <v>0.56259338999999997</v>
       </c>
-      <c r="BN49">
+      <c r="BO49">
         <v>0.56553142599999995</v>
       </c>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -37241,14 +37392,17 @@
         <v>-0.75955798200000002</v>
       </c>
       <c r="BM50">
+        <v>-0.75947107883331599</v>
+      </c>
+      <c r="BN50">
         <f t="shared" si="12"/>
         <v>0.75955798200000002</v>
       </c>
-      <c r="BN50">
+      <c r="BO50">
         <v>0.51736134499999997</v>
       </c>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -37460,14 +37614,17 @@
         <v>-0.60147586200000003</v>
       </c>
       <c r="BM51">
+        <v>-0.67489285175272296</v>
+      </c>
+      <c r="BN51">
         <f t="shared" si="12"/>
         <v>0.60147586200000003</v>
       </c>
-      <c r="BN51">
+      <c r="BO51">
         <v>0.46425909599999998</v>
       </c>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -37679,14 +37836,17 @@
         <v>-0.69149139500000001</v>
       </c>
       <c r="BM52">
+        <v>-0.70016460937340097</v>
+      </c>
+      <c r="BN52">
         <f t="shared" si="12"/>
         <v>0.69149139500000001</v>
       </c>
-      <c r="BN52">
+      <c r="BO52">
         <v>0.56460365300000004</v>
       </c>
     </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -37898,14 +38058,17 @@
         <v>-0.49252285800000001</v>
       </c>
       <c r="BM53">
+        <v>-0.59115402731607303</v>
+      </c>
+      <c r="BN53">
         <f t="shared" si="12"/>
         <v>0.49252285800000001</v>
       </c>
-      <c r="BN53">
+      <c r="BO53">
         <v>0.57628232800000001</v>
       </c>
     </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -38117,14 +38280,17 @@
         <v>-0.649723567</v>
       </c>
       <c r="BM54">
+        <v>-0.68182926841287295</v>
+      </c>
+      <c r="BN54">
         <f t="shared" si="12"/>
         <v>0.649723567</v>
       </c>
-      <c r="BN54">
+      <c r="BO54">
         <v>0.53162991199999998</v>
       </c>
     </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -38336,14 +38502,17 @@
         <v>-0.59026629100000005</v>
       </c>
       <c r="BM55">
+        <v>-0.63693130722312497</v>
+      </c>
+      <c r="BN55">
         <f t="shared" si="12"/>
         <v>0.59026629100000005</v>
       </c>
-      <c r="BN55">
+      <c r="BO55">
         <v>0.451402953</v>
       </c>
     </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -38555,14 +38724,17 @@
         <v>-0.877291504</v>
       </c>
       <c r="BM56">
+        <v>-0.91739336267348903</v>
+      </c>
+      <c r="BN56">
         <f t="shared" si="12"/>
         <v>0.877291504</v>
       </c>
-      <c r="BN56">
+      <c r="BO56">
         <v>0.379192001</v>
       </c>
     </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -38774,14 +38946,17 @@
         <v>-0.77358954099999999</v>
       </c>
       <c r="BM57">
+        <v>-0.82127018437088095</v>
+      </c>
+      <c r="BN57">
         <f t="shared" si="12"/>
         <v>0.77358954099999999</v>
       </c>
-      <c r="BN57">
+      <c r="BO57">
         <v>0.71935892800000001</v>
       </c>
     </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -38993,14 +39168,17 @@
         <v>-0.66050697400000002</v>
       </c>
       <c r="BM58">
+        <v>-0.68057870936131004</v>
+      </c>
+      <c r="BN58">
         <f t="shared" si="12"/>
         <v>0.66050697400000002</v>
       </c>
-      <c r="BN58">
+      <c r="BO58">
         <v>0.37918802299999999</v>
       </c>
     </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -39212,14 +39390,17 @@
         <v>-0.69503941800000002</v>
       </c>
       <c r="BM59">
+        <v>-0.71206542584020704</v>
+      </c>
+      <c r="BN59">
         <f t="shared" si="12"/>
         <v>0.69503941800000002</v>
       </c>
-      <c r="BN59">
+      <c r="BO59">
         <v>0.53146045099999994</v>
       </c>
     </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -39431,14 +39612,17 @@
         <v>-0.74356962500000001</v>
       </c>
       <c r="BM60">
+        <v>-0.76523146256757901</v>
+      </c>
+      <c r="BN60">
         <f t="shared" si="12"/>
         <v>0.74356962500000001</v>
       </c>
-      <c r="BN60">
+      <c r="BO60">
         <v>0.68960581499999996</v>
       </c>
     </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -39650,14 +39834,17 @@
         <v>-0.67909167699999995</v>
       </c>
       <c r="BM61">
+        <v>-0.70152405908242399</v>
+      </c>
+      <c r="BN61">
         <f t="shared" si="12"/>
         <v>0.67909167699999995</v>
       </c>
-      <c r="BN61">
+      <c r="BO61">
         <v>0.68960581499999996</v>
       </c>
     </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -39869,14 +40056,17 @@
         <v>-0.71511798800000004</v>
       </c>
       <c r="BM62">
+        <v>-0.72707287413829602</v>
+      </c>
+      <c r="BN62">
         <f t="shared" si="12"/>
         <v>0.71511798800000004</v>
       </c>
-      <c r="BN62">
+      <c r="BO62">
         <v>0.68960581499999996</v>
       </c>
     </row>
-    <row r="63" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -40088,14 +40278,17 @@
         <v>-0.71070357699999998</v>
       </c>
       <c r="BM63">
+        <v>-0.73434896166725805</v>
+      </c>
+      <c r="BN63">
         <f t="shared" si="12"/>
         <v>0.71070357699999998</v>
       </c>
-      <c r="BN63">
+      <c r="BO63">
         <v>0.46280822300000002</v>
       </c>
     </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -40307,14 +40500,17 @@
         <v>-0.73094808200000005</v>
       </c>
       <c r="BM64">
+        <v>-0.76314961475425103</v>
+      </c>
+      <c r="BN64">
         <f t="shared" si="12"/>
         <v>0.73094808200000005</v>
       </c>
-      <c r="BN64">
+      <c r="BO64">
         <v>0.53526619399999997</v>
       </c>
     </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -40526,14 +40722,17 @@
         <v>-0.68829276100000003</v>
       </c>
       <c r="BM65">
+        <v>-0.73882239758798296</v>
+      </c>
+      <c r="BN65">
         <f t="shared" si="12"/>
         <v>0.68829276100000003</v>
       </c>
-      <c r="BN65">
+      <c r="BO65">
         <v>0.53581091599999997</v>
       </c>
     </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -40745,14 +40944,17 @@
         <v>-0.76379462099999995</v>
       </c>
       <c r="BM66">
+        <v>-0.75839668277130801</v>
+      </c>
+      <c r="BN66">
         <f t="shared" si="12"/>
         <v>0.76379462099999995</v>
       </c>
-      <c r="BN66">
+      <c r="BO66">
         <v>0.52562926099999996</v>
       </c>
     </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -40964,14 +41166,17 @@
         <v>-0.87719946900000001</v>
       </c>
       <c r="BM67">
-        <f t="shared" ref="BM67:BM114" si="25">-BL67</f>
+        <v>-0.88822182776738701</v>
+      </c>
+      <c r="BN67">
+        <f t="shared" ref="BN67:BN114" si="25">-BL67</f>
         <v>0.87719946900000001</v>
       </c>
-      <c r="BN67">
+      <c r="BO67">
         <v>0.64766716700000004</v>
       </c>
     </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -41183,14 +41388,17 @@
         <v>-0.84588698900000003</v>
       </c>
       <c r="BM68">
+        <v>-0.861311613642611</v>
+      </c>
+      <c r="BN68">
         <f t="shared" si="25"/>
         <v>0.84588698900000003</v>
       </c>
-      <c r="BN68">
+      <c r="BO68">
         <v>0.52562926099999996</v>
       </c>
     </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -41402,14 +41610,17 @@
         <v>-0.66001782799999997</v>
       </c>
       <c r="BM69">
+        <v>-0.59658008456351797</v>
+      </c>
+      <c r="BN69">
         <f t="shared" si="25"/>
         <v>0.66001782799999997</v>
       </c>
-      <c r="BN69">
+      <c r="BO69">
         <v>0.52711257199999995</v>
       </c>
     </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -41621,14 +41832,17 @@
         <v>-0.68679993399999995</v>
       </c>
       <c r="BM70">
+        <v>-0.68586128806916002</v>
+      </c>
+      <c r="BN70">
         <f t="shared" si="25"/>
         <v>0.68679993399999995</v>
       </c>
-      <c r="BN70">
+      <c r="BO70">
         <v>0.58060979599999996</v>
       </c>
     </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -41840,14 +42054,17 @@
         <v>-0.64383950199999995</v>
       </c>
       <c r="BM71">
+        <v>-0.73254649392720905</v>
+      </c>
+      <c r="BN71">
         <f t="shared" si="25"/>
         <v>0.64383950199999995</v>
       </c>
-      <c r="BN71">
+      <c r="BO71">
         <v>0.68960581499999996</v>
       </c>
     </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -42059,14 +42276,17 @@
         <v>-0.74030450199999998</v>
       </c>
       <c r="BM72">
+        <v>-0.77130346572170205</v>
+      </c>
+      <c r="BN72">
         <f t="shared" si="25"/>
         <v>0.74030450199999998</v>
       </c>
-      <c r="BN72">
+      <c r="BO72">
         <v>0.53162991199999998</v>
       </c>
     </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -42278,14 +42498,17 @@
         <v>-0.56799372800000003</v>
       </c>
       <c r="BM73">
+        <v>-0.60276783380205601</v>
+      </c>
+      <c r="BN73">
         <f t="shared" si="25"/>
         <v>0.56799372800000003</v>
       </c>
-      <c r="BN73">
+      <c r="BO73">
         <v>0.41672614800000002</v>
       </c>
     </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -42497,14 +42720,17 @@
         <v>-0.65860930500000003</v>
       </c>
       <c r="BM74">
+        <v>-0.64018512138341399</v>
+      </c>
+      <c r="BN74">
         <f t="shared" si="25"/>
         <v>0.65860930500000003</v>
       </c>
-      <c r="BN74">
+      <c r="BO74">
         <v>0.57958336399999999</v>
       </c>
     </row>
-    <row r="75" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -42716,14 +42942,17 @@
         <v>-0.72675799200000002</v>
       </c>
       <c r="BM75">
+        <v>-0.72853001460093603</v>
+      </c>
+      <c r="BN75">
         <f t="shared" si="25"/>
         <v>0.72675799200000002</v>
       </c>
-      <c r="BN75">
+      <c r="BO75">
         <v>0.51736134499999997</v>
       </c>
     </row>
-    <row r="76" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -42935,14 +43164,17 @@
         <v>-0.42794660200000001</v>
       </c>
       <c r="BM76">
+        <v>-0.53808256765509499</v>
+      </c>
+      <c r="BN76">
         <f t="shared" si="25"/>
         <v>0.42794660200000001</v>
       </c>
-      <c r="BN76">
+      <c r="BO76">
         <v>0.451402953</v>
       </c>
     </row>
-    <row r="77" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -43154,14 +43386,17 @@
         <v>-0.77784398600000004</v>
       </c>
       <c r="BM77">
+        <v>-0.78049439600147996</v>
+      </c>
+      <c r="BN77">
         <f t="shared" si="25"/>
         <v>0.77784398600000004</v>
       </c>
-      <c r="BN77">
+      <c r="BO77">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="78" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -43373,14 +43608,17 @@
         <v>-0.56028331399999998</v>
       </c>
       <c r="BM78">
+        <v>-0.480257633369853</v>
+      </c>
+      <c r="BN78">
         <f t="shared" si="25"/>
         <v>0.56028331399999998</v>
       </c>
-      <c r="BN78">
+      <c r="BO78">
         <v>0.50351591900000003</v>
       </c>
     </row>
-    <row r="79" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -43592,14 +43830,17 @@
         <v>-0.71794897499999999</v>
       </c>
       <c r="BM79">
+        <v>-0.75457445924239597</v>
+      </c>
+      <c r="BN79">
         <f t="shared" si="25"/>
         <v>0.71794897499999999</v>
       </c>
-      <c r="BN79">
+      <c r="BO79">
         <v>0.68960581499999996</v>
       </c>
     </row>
-    <row r="80" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -43811,14 +44052,17 @@
         <v>-0.78434057000000001</v>
       </c>
       <c r="BM80">
+        <v>-0.78840559431781199</v>
+      </c>
+      <c r="BN80">
         <f t="shared" si="25"/>
         <v>0.78434057000000001</v>
       </c>
-      <c r="BN80">
+      <c r="BO80">
         <v>0.61497841200000003</v>
       </c>
     </row>
-    <row r="81" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -44030,14 +44274,17 @@
         <v>-0.92187818899999996</v>
       </c>
       <c r="BM81">
+        <v>-0.88528648448121705</v>
+      </c>
+      <c r="BN81">
         <f t="shared" si="25"/>
         <v>0.92187818899999996</v>
       </c>
-      <c r="BN81">
+      <c r="BO81">
         <v>0.64766716700000004</v>
       </c>
     </row>
-    <row r="82" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -44249,14 +44496,17 @@
         <v>-0.40468551000000003</v>
       </c>
       <c r="BM82">
+        <v>-0.530944243124989</v>
+      </c>
+      <c r="BN82">
         <f t="shared" si="25"/>
         <v>0.40468551000000003</v>
       </c>
-      <c r="BN82">
+      <c r="BO82">
         <v>0.52032293100000004</v>
       </c>
     </row>
-    <row r="83" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -44468,14 +44718,17 @@
         <v>-0.765910062</v>
       </c>
       <c r="BM83">
+        <v>-0.80162078635278</v>
+      </c>
+      <c r="BN83">
         <f t="shared" si="25"/>
         <v>0.765910062</v>
       </c>
-      <c r="BN83">
+      <c r="BO83">
         <v>0.47942077599999999</v>
       </c>
     </row>
-    <row r="84" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -44687,14 +44940,17 @@
         <v>-0.63977804100000002</v>
       </c>
       <c r="BM84">
+        <v>-0.70723247095284103</v>
+      </c>
+      <c r="BN84">
         <f t="shared" si="25"/>
         <v>0.63977804100000002</v>
       </c>
-      <c r="BN84">
+      <c r="BO84">
         <v>0.41256108600000002</v>
       </c>
     </row>
-    <row r="85" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -44906,14 +45162,17 @@
         <v>-0.59807737999999999</v>
       </c>
       <c r="BM85">
+        <v>-0.64820564445245199</v>
+      </c>
+      <c r="BN85">
         <f t="shared" si="25"/>
         <v>0.59807737999999999</v>
       </c>
-      <c r="BN85">
+      <c r="BO85">
         <v>0.40215384900000001</v>
       </c>
     </row>
-    <row r="86" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -45125,14 +45384,17 @@
         <v>-0.775809321</v>
       </c>
       <c r="BM86">
+        <v>-0.78991556536441498</v>
+      </c>
+      <c r="BN86">
         <f t="shared" si="25"/>
         <v>0.775809321</v>
       </c>
-      <c r="BN86">
+      <c r="BO86">
         <v>0.56869322499999997</v>
       </c>
     </row>
-    <row r="87" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -45344,14 +45606,17 @@
         <v>-0.81720079800000001</v>
       </c>
       <c r="BM87">
+        <v>-0.81740505066540203</v>
+      </c>
+      <c r="BN87">
         <f t="shared" si="25"/>
         <v>0.81720079800000001</v>
       </c>
-      <c r="BN87">
+      <c r="BO87">
         <v>0.59108196700000004</v>
       </c>
     </row>
-    <row r="88" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -45563,14 +45828,17 @@
         <v>-0.70468253999999997</v>
       </c>
       <c r="BM88">
+        <v>-0.70291925745766304</v>
+      </c>
+      <c r="BN88">
         <f t="shared" si="25"/>
         <v>0.70468253999999997</v>
       </c>
-      <c r="BN88">
+      <c r="BO88">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="89" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -45782,14 +46050,17 @@
         <v>-0.79704902499999997</v>
       </c>
       <c r="BM89">
+        <v>-0.85705388171658603</v>
+      </c>
+      <c r="BN89">
         <f t="shared" si="25"/>
         <v>0.79704902499999997</v>
       </c>
-      <c r="BN89">
+      <c r="BO89">
         <v>0.50925102300000002</v>
       </c>
     </row>
-    <row r="90" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -46001,14 +46272,17 @@
         <v>-0.60188481199999999</v>
       </c>
       <c r="BM90">
+        <v>-0.62375340896610199</v>
+      </c>
+      <c r="BN90">
         <f t="shared" si="25"/>
         <v>0.60188481199999999</v>
       </c>
-      <c r="BN90">
+      <c r="BO90">
         <v>0.50351591900000003</v>
       </c>
     </row>
-    <row r="91" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -46220,14 +46494,17 @@
         <v>-0.58839604300000004</v>
       </c>
       <c r="BM91">
+        <v>-0.56898273540757605</v>
+      </c>
+      <c r="BN91">
         <f t="shared" si="25"/>
         <v>0.58839604300000004</v>
       </c>
-      <c r="BN91">
+      <c r="BO91">
         <v>0.50351591900000003</v>
       </c>
     </row>
-    <row r="92" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -46439,14 +46716,17 @@
         <v>-0.68228940699999996</v>
       </c>
       <c r="BM92">
+        <v>-0.68811251016804698</v>
+      </c>
+      <c r="BN92">
         <f t="shared" si="25"/>
         <v>0.68228940699999996</v>
       </c>
-      <c r="BN92">
+      <c r="BO92">
         <v>0.53949475300000005</v>
       </c>
     </row>
-    <row r="93" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -46658,14 +46938,17 @@
         <v>-0.57920705800000005</v>
       </c>
       <c r="BM93">
+        <v>-0.71354488406040895</v>
+      </c>
+      <c r="BN93">
         <f t="shared" si="25"/>
         <v>0.57920705800000005</v>
       </c>
-      <c r="BN93">
+      <c r="BO93">
         <v>0.44607749699999999</v>
       </c>
     </row>
-    <row r="94" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -46877,14 +47160,17 @@
         <v>-0.55864167200000003</v>
       </c>
       <c r="BM94">
+        <v>-0.58590258776976101</v>
+      </c>
+      <c r="BN94">
         <f t="shared" si="25"/>
         <v>0.55864167200000003</v>
       </c>
-      <c r="BN94">
+      <c r="BO94">
         <v>0.53762866799999998</v>
       </c>
     </row>
-    <row r="95" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -47096,14 +47382,17 @@
         <v>-0.76199160300000002</v>
       </c>
       <c r="BM95">
+        <v>-0.74591205323381404</v>
+      </c>
+      <c r="BN95">
         <f t="shared" si="25"/>
         <v>0.76199160300000002</v>
       </c>
-      <c r="BN95">
+      <c r="BO95">
         <v>0.61497841200000003</v>
       </c>
     </row>
-    <row r="96" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -47315,14 +47604,17 @@
         <v>-0.68675508500000004</v>
       </c>
       <c r="BM96">
+        <v>-0.72220675607559903</v>
+      </c>
+      <c r="BN96">
         <f t="shared" si="25"/>
         <v>0.68675508500000004</v>
       </c>
-      <c r="BN96">
+      <c r="BO96">
         <v>0.52022376999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -47534,14 +47826,17 @@
         <v>-0.60134855300000001</v>
       </c>
       <c r="BM97">
+        <v>-0.62307607616301397</v>
+      </c>
+      <c r="BN97">
         <f t="shared" si="25"/>
         <v>0.60134855300000001</v>
       </c>
-      <c r="BN97">
+      <c r="BO97">
         <v>0.53762866799999998</v>
       </c>
     </row>
-    <row r="98" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -47753,14 +48048,17 @@
         <v>-0.64682027600000003</v>
       </c>
       <c r="BM98">
+        <v>-0.707152907386703</v>
+      </c>
+      <c r="BN98">
         <f t="shared" si="25"/>
         <v>0.64682027600000003</v>
       </c>
-      <c r="BN98">
+      <c r="BO98">
         <v>0.49834260499999999</v>
       </c>
     </row>
-    <row r="99" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -47972,14 +48270,17 @@
         <v>-0.90434851999999999</v>
       </c>
       <c r="BM99">
+        <v>-0.92858530594068001</v>
+      </c>
+      <c r="BN99">
         <f t="shared" si="25"/>
         <v>0.90434851999999999</v>
       </c>
-      <c r="BN99">
+      <c r="BO99">
         <v>0.62417910399999998</v>
       </c>
     </row>
-    <row r="100" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -48191,14 +48492,17 @@
         <v>-1.0237219369999999</v>
       </c>
       <c r="BM100">
+        <v>-0.97905414518513001</v>
+      </c>
+      <c r="BN100">
         <f t="shared" si="25"/>
         <v>1.0237219369999999</v>
       </c>
-      <c r="BN100">
+      <c r="BO100">
         <v>0.48291107</v>
       </c>
     </row>
-    <row r="101" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -48410,14 +48714,17 @@
         <v>-0.98120611300000005</v>
       </c>
       <c r="BM101">
+        <v>-0.97873800885010098</v>
+      </c>
+      <c r="BN101">
         <f t="shared" si="25"/>
         <v>0.98120611300000005</v>
       </c>
-      <c r="BN101">
+      <c r="BO101">
         <v>0.62358948700000005</v>
       </c>
     </row>
-    <row r="102" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -48629,14 +48936,17 @@
         <v>-0.76810126599999995</v>
       </c>
       <c r="BM102">
+        <v>-0.78292428836845895</v>
+      </c>
+      <c r="BN102">
         <f t="shared" si="25"/>
         <v>0.76810126599999995</v>
       </c>
-      <c r="BN102">
+      <c r="BO102">
         <v>0.48850552699999999</v>
       </c>
     </row>
-    <row r="103" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>108</v>
       </c>
@@ -48848,14 +49158,17 @@
         <v>-0.71557703399999995</v>
       </c>
       <c r="BM103">
+        <v>-0.70931207549233399</v>
+      </c>
+      <c r="BN103">
         <f t="shared" si="25"/>
         <v>0.71557703399999995</v>
       </c>
-      <c r="BN103">
+      <c r="BO103">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="104" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>109</v>
       </c>
@@ -49067,14 +49380,17 @@
         <v>-0.73733957000000006</v>
       </c>
       <c r="BM104">
+        <v>-0.75554439045586896</v>
+      </c>
+      <c r="BN104">
         <f t="shared" si="25"/>
         <v>0.73733957000000006</v>
       </c>
-      <c r="BN104">
+      <c r="BO104">
         <v>0.56623688500000002</v>
       </c>
     </row>
-    <row r="105" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>110</v>
       </c>
@@ -49286,14 +49602,17 @@
         <v>-0.42053823600000001</v>
       </c>
       <c r="BM105">
+        <v>-0.51662942743434004</v>
+      </c>
+      <c r="BN105">
         <f t="shared" si="25"/>
         <v>0.42053823600000001</v>
       </c>
-      <c r="BN105">
+      <c r="BO105">
         <v>0.451402953</v>
       </c>
     </row>
-    <row r="106" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -49505,14 +49824,17 @@
         <v>-1.045262296</v>
       </c>
       <c r="BM106">
+        <v>-1.0074088614115699</v>
+      </c>
+      <c r="BN106">
         <f t="shared" si="25"/>
         <v>1.045262296</v>
       </c>
-      <c r="BN106">
+      <c r="BO106">
         <v>0.62358948700000005</v>
       </c>
     </row>
-    <row r="107" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>112</v>
       </c>
@@ -49724,14 +50046,17 @@
         <v>-0.96387067900000001</v>
       </c>
       <c r="BM107">
+        <v>-0.96997454916736703</v>
+      </c>
+      <c r="BN107">
         <f t="shared" si="25"/>
         <v>0.96387067900000001</v>
       </c>
-      <c r="BN107">
+      <c r="BO107">
         <v>0.59318082599999999</v>
       </c>
     </row>
-    <row r="108" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>113</v>
       </c>
@@ -49943,14 +50268,17 @@
         <v>-0.75805058599999997</v>
       </c>
       <c r="BM108">
+        <v>-0.74459160120467305</v>
+      </c>
+      <c r="BN108">
         <f t="shared" si="25"/>
         <v>0.75805058599999997</v>
       </c>
-      <c r="BN108">
+      <c r="BO108">
         <v>0.53623771499999995</v>
       </c>
     </row>
-    <row r="109" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>114</v>
       </c>
@@ -50162,14 +50490,17 @@
         <v>-0.59263524499999998</v>
       </c>
       <c r="BM109">
+        <v>-0.61709152583053295</v>
+      </c>
+      <c r="BN109">
         <f t="shared" si="25"/>
         <v>0.59263524499999998</v>
       </c>
-      <c r="BN109">
+      <c r="BO109">
         <v>0.51135295400000003</v>
       </c>
     </row>
-    <row r="110" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>115</v>
       </c>
@@ -50381,14 +50712,17 @@
         <v>-0.48370160699999998</v>
       </c>
       <c r="BM110">
+        <v>-0.477667844015771</v>
+      </c>
+      <c r="BN110">
         <f t="shared" si="25"/>
         <v>0.48370160699999998</v>
       </c>
-      <c r="BN110">
+      <c r="BO110">
         <v>0.48345510400000002</v>
       </c>
     </row>
-    <row r="111" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>116</v>
       </c>
@@ -50600,14 +50934,17 @@
         <v>-0.96651553099999998</v>
       </c>
       <c r="BM111">
+        <v>-0.96186476450653902</v>
+      </c>
+      <c r="BN111">
         <f t="shared" si="25"/>
         <v>0.96651553099999998</v>
       </c>
-      <c r="BN111">
+      <c r="BO111">
         <v>0.56869322499999997</v>
       </c>
     </row>
-    <row r="112" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>117</v>
       </c>
@@ -50819,14 +51156,17 @@
         <v>-0.77528207800000004</v>
       </c>
       <c r="BM112">
+        <v>-0.81268189999523499</v>
+      </c>
+      <c r="BN112">
         <f t="shared" si="25"/>
         <v>0.77528207800000004</v>
       </c>
-      <c r="BN112">
+      <c r="BO112">
         <v>0.62027838199999996</v>
       </c>
     </row>
-    <row r="113" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>118</v>
       </c>
@@ -51038,14 +51378,17 @@
         <v>-0.81886512</v>
       </c>
       <c r="BM113">
+        <v>-0.83180650577801896</v>
+      </c>
+      <c r="BN113">
         <f t="shared" si="25"/>
         <v>0.81886512</v>
       </c>
-      <c r="BN113">
+      <c r="BO113">
         <v>0.49090901300000001</v>
       </c>
     </row>
-    <row r="114" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>119</v>
       </c>
@@ -51257,10 +51600,13 @@
         <v>-0.70824022200000003</v>
       </c>
       <c r="BM114">
+        <v>-0.76476613867983101</v>
+      </c>
+      <c r="BN114">
         <f t="shared" si="25"/>
         <v>0.70824022200000003</v>
       </c>
-      <c r="BN114">
+      <c r="BO114">
         <v>0.71935892800000001</v>
       </c>
     </row>

</xml_diff>